<commit_message>
Education Return was corrected Skills Months was added but in testing phase
</commit_message>
<xml_diff>
--- a/upload_files/BK_746_2-converted__text.xlsx
+++ b/upload_files/BK_746_2-converted__text.xlsx
@@ -613,19 +613,19 @@
     <t>embedded software : 1</t>
   </si>
   <si>
+    <t>git : 1</t>
+  </si>
+  <si>
     <t>project : 1</t>
   </si>
   <si>
     <t>sql : 1</t>
   </si>
   <si>
+    <t>databases : 2</t>
+  </si>
+  <si>
     <t>analysis : 1</t>
-  </si>
-  <si>
-    <t>databases : 2</t>
-  </si>
-  <si>
-    <t>git : 1</t>
   </si>
   <si>
     <t>35.71</t>

</xml_diff>

<commit_message>
Debugs were removed Monthly Skills were added
</commit_message>
<xml_diff>
--- a/upload_files/BK_746_2-converted__text.xlsx
+++ b/upload_files/BK_746_2-converted__text.xlsx
@@ -613,16 +613,16 @@
     <t>embedded software : 1</t>
   </si>
   <si>
+    <t>databases : 2</t>
+  </si>
+  <si>
     <t>git : 1</t>
   </si>
   <si>
+    <t>sql : 1</t>
+  </si>
+  <si>
     <t>project : 1</t>
-  </si>
-  <si>
-    <t>sql : 1</t>
-  </si>
-  <si>
-    <t>databases : 2</t>
   </si>
   <si>
     <t>analysis : 1</t>

</xml_diff>

<commit_message>
2 word skills are analysed as well
</commit_message>
<xml_diff>
--- a/upload_files/BK_746_2-converted__text.xlsx
+++ b/upload_files/BK_746_2-converted__text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="240">
   <si>
     <t>CV ID</t>
   </si>
@@ -55,7 +55,10 @@
     <t>text.txt</t>
   </si>
   <si>
-    <t>33.76</t>
+    <t>26.80</t>
+  </si>
+  <si>
+    <t>image processing : 1</t>
   </si>
   <si>
     <t>communications : 1</t>
@@ -76,19 +79,22 @@
     <t>tv : 2</t>
   </si>
   <si>
+    <t>financial services : 3</t>
+  </si>
+  <si>
     <t>international : 2</t>
   </si>
   <si>
-    <t>network : 14</t>
-  </si>
-  <si>
-    <t>systems : 14</t>
+    <t>network : 8</t>
+  </si>
+  <si>
+    <t>systems : 12</t>
   </si>
   <si>
     <t>telecommunications : 3</t>
   </si>
   <si>
-    <t>oracle : 200</t>
+    <t>oracle dba : 53</t>
   </si>
   <si>
     <t>dba : 73</t>
@@ -97,7 +103,10 @@
     <t>consultant : 8</t>
   </si>
   <si>
-    <t>unix : 12</t>
+    <t>unix : 7</t>
+  </si>
+  <si>
+    <t>system administrator : 7</t>
   </si>
   <si>
     <t>administrator : 5</t>
@@ -115,6 +124,12 @@
     <t>admin : 1</t>
   </si>
   <si>
+    <t>oracle : 130</t>
+  </si>
+  <si>
+    <t>oracle applications : 3</t>
+  </si>
+  <si>
     <t>middleware : 4</t>
   </si>
   <si>
@@ -124,6 +139,9 @@
     <t>monitor : 1</t>
   </si>
   <si>
+    <t>oracle databases : 8</t>
+  </si>
+  <si>
     <t>databases : 28</t>
   </si>
   <si>
@@ -142,7 +160,7 @@
     <t>testing : 10</t>
   </si>
   <si>
-    <t>redhat : 9</t>
+    <t>redhat linux : 16</t>
   </si>
   <si>
     <t>linux : 14</t>
@@ -166,7 +184,7 @@
     <t>tools : 3</t>
   </si>
   <si>
-    <t>database : 31</t>
+    <t>database : 29</t>
   </si>
   <si>
     <t>backup : 7</t>
@@ -175,12 +193,15 @@
     <t>recovery : 5</t>
   </si>
   <si>
-    <t>production : 18</t>
+    <t>production : 15</t>
   </si>
   <si>
     <t>development : 21</t>
   </si>
   <si>
+    <t>production support : 5</t>
+  </si>
+  <si>
     <t>ibm : 6</t>
   </si>
   <si>
@@ -193,13 +214,16 @@
     <t>azure : 1</t>
   </si>
   <si>
+    <t>oracle 12c : 9</t>
+  </si>
+  <si>
     <t>rac : 29</t>
   </si>
   <si>
     <t>node : 1</t>
   </si>
   <si>
-    <t>security : 10</t>
+    <t>security : 6</t>
   </si>
   <si>
     <t>installation : 8</t>
@@ -208,7 +232,13 @@
     <t>soa : 2</t>
   </si>
   <si>
-    <t>windows : 11</t>
+    <t>performance monitoring : 2</t>
+  </si>
+  <si>
+    <t>windows : 7</t>
+  </si>
+  <si>
+    <t>database management : 1</t>
   </si>
   <si>
     <t>management : 24</t>
@@ -217,13 +247,16 @@
     <t>sales : 2</t>
   </si>
   <si>
+    <t>oracle rac : 6</t>
+  </si>
+  <si>
     <t>symantec : 2</t>
   </si>
   <si>
     <t>automated : 1</t>
   </si>
   <si>
-    <t>configuration : 17</t>
+    <t>configuration : 16</t>
   </si>
   <si>
     <t>sqlserver : 5</t>
@@ -232,19 +265,25 @@
     <t>training : 5</t>
   </si>
   <si>
-    <t>sql : 17</t>
+    <t>sql : 12</t>
   </si>
   <si>
     <t>rackspace : 2</t>
   </si>
   <si>
-    <t>aws : 6</t>
+    <t>aws : 5</t>
+  </si>
+  <si>
+    <t>oracle database : 6</t>
   </si>
   <si>
     <t>warehouse : 2</t>
   </si>
   <si>
-    <t>cloud : 2</t>
+    <t>aws cloud : 1</t>
+  </si>
+  <si>
+    <t>cloud computing : 2</t>
   </si>
   <si>
     <t>informatica : 4</t>
@@ -262,15 +301,30 @@
     <t>toad : 6</t>
   </si>
   <si>
+    <t>sql tuning : 5</t>
+  </si>
+  <si>
+    <t>windows servers : 4</t>
+  </si>
+  <si>
+    <t>red hat : 2</t>
+  </si>
+  <si>
     <t>rest : 1</t>
   </si>
   <si>
+    <t>unix scripting : 4</t>
+  </si>
+  <si>
     <t>scripting : 6</t>
   </si>
   <si>
     <t>powershell : 1</t>
   </si>
   <si>
+    <t>elastic search : 2</t>
+  </si>
+  <si>
     <t>git : 2</t>
   </si>
   <si>
@@ -292,12 +346,27 @@
     <t>ux : 1</t>
   </si>
   <si>
+    <t>oracle sql : 2</t>
+  </si>
+  <si>
+    <t>sql server : 1</t>
+  </si>
+  <si>
+    <t>high availability : 4</t>
+  </si>
+  <si>
+    <t>data quality : 2</t>
+  </si>
+  <si>
     <t>audit : 4</t>
   </si>
   <si>
     <t>regulations : 1</t>
   </si>
   <si>
+    <t>data architect : 1</t>
+  </si>
+  <si>
     <t>architect : 1</t>
   </si>
   <si>
@@ -307,25 +376,40 @@
     <t>analysis : 11</t>
   </si>
   <si>
+    <t>sql dba : 1</t>
+  </si>
+  <si>
     <t>solaris : 10</t>
   </si>
   <si>
+    <t>cloud : 1</t>
+  </si>
+  <si>
     <t>weblogic : 2</t>
   </si>
   <si>
     <t>apex : 2</t>
   </si>
   <si>
+    <t>performance tuning : 2</t>
+  </si>
+  <si>
+    <t>data migration : 1</t>
+  </si>
+  <si>
     <t>tde : 1</t>
   </si>
   <si>
+    <t>data encryption : 1</t>
+  </si>
+  <si>
     <t>encryption : 1</t>
   </si>
   <si>
     <t>perl : 2</t>
   </si>
   <si>
-    <t>shell : 3</t>
+    <t>shell : 2</t>
   </si>
   <si>
     <t>virtualization : 3</t>
@@ -337,21 +421,36 @@
     <t>asm : 9</t>
   </si>
   <si>
+    <t>stored procedures : 1</t>
+  </si>
+  <si>
     <t>tables : 1</t>
   </si>
   <si>
     <t>pci : 1</t>
   </si>
   <si>
+    <t>security clearance : 5</t>
+  </si>
+  <si>
+    <t>oracle fusion : 2</t>
+  </si>
+  <si>
     <t>fusion : 1</t>
   </si>
   <si>
     <t>scheduling : 1</t>
   </si>
   <si>
+    <t>configuration management : 1</t>
+  </si>
+  <si>
     <t>remedy : 2</t>
   </si>
   <si>
+    <t>incident management : 1</t>
+  </si>
+  <si>
     <t>sla : 2</t>
   </si>
   <si>
@@ -367,6 +466,9 @@
     <t>engineering : 1</t>
   </si>
   <si>
+    <t>ms sql : 1</t>
+  </si>
+  <si>
     <t>bi : 2</t>
   </si>
   <si>
@@ -382,9 +484,18 @@
     <t>documentation : 2</t>
   </si>
   <si>
+    <t>unix shell : 1</t>
+  </si>
+  <si>
+    <t>shell scripting : 1</t>
+  </si>
+  <si>
     <t>mis : 1</t>
   </si>
   <si>
+    <t>data capture : 2</t>
+  </si>
+  <si>
     <t>similar : 1</t>
   </si>
   <si>
@@ -394,6 +505,12 @@
     <t>forecasting : 1</t>
   </si>
   <si>
+    <t>capital market : 1</t>
+  </si>
+  <si>
+    <t>market research : 1</t>
+  </si>
+  <si>
     <t>research : 1</t>
   </si>
   <si>
@@ -403,6 +520,12 @@
     <t>operations : 2</t>
   </si>
   <si>
+    <t>database tuning : 2</t>
+  </si>
+  <si>
+    <t>trouble shooting : 2</t>
+  </si>
+  <si>
     <t>statistics : 1</t>
   </si>
   <si>
@@ -418,217 +541,190 @@
     <t>emc : 3</t>
   </si>
   <si>
+    <t>data warehousing : 1</t>
+  </si>
+  <si>
+    <t>disaster recovery : 3</t>
+  </si>
+  <si>
     <t>reporting : 2</t>
   </si>
   <si>
     <t>veritas : 4</t>
   </si>
   <si>
+    <t>windows server : 2</t>
+  </si>
+  <si>
+    <t>credit risk : 1</t>
+  </si>
+  <si>
+    <t>risk assessment : 1</t>
+  </si>
+  <si>
+    <t>general ledger : 2</t>
+  </si>
+  <si>
     <t>peoplesoft : 1</t>
   </si>
   <si>
     <t>sybase : 1</t>
   </si>
   <si>
-    <t>software : 11</t>
+    <t>software : 9</t>
+  </si>
+  <si>
+    <t>enterprise manager : 2</t>
   </si>
   <si>
     <t>pl : 2</t>
   </si>
   <si>
+    <t>system administration : 3</t>
+  </si>
+  <si>
     <t>apache : 2</t>
   </si>
   <si>
+    <t>business objects : 2</t>
+  </si>
+  <si>
+    <t>business continuity : 1</t>
+  </si>
+  <si>
     <t>cluster : 6</t>
   </si>
   <si>
+    <t>quality assurance : 1</t>
+  </si>
+  <si>
     <t>os : 1</t>
   </si>
   <si>
     <t>tivoli : 2</t>
   </si>
   <si>
+    <t>network management : 7</t>
+  </si>
+  <si>
     <t>tcp : 3</t>
   </si>
   <si>
     <t>ip : 3</t>
   </si>
   <si>
-    <t>cisco : 1</t>
+    <t>cisco routers : 2</t>
   </si>
   <si>
     <t>routers : 2</t>
   </si>
   <si>
+    <t>network security : 1</t>
+  </si>
+  <si>
+    <t>security policies : 1</t>
+  </si>
+  <si>
     <t>policies : 1</t>
   </si>
   <si>
     <t>vms : 4</t>
   </si>
   <si>
+    <t>unix administration : 1</t>
+  </si>
+  <si>
     <t>c : 2</t>
   </si>
   <si>
     <t>communication : 1</t>
   </si>
   <si>
+    <t>system analysis : 2</t>
+  </si>
+  <si>
     <t>integration : 2</t>
   </si>
   <si>
+    <t>customer support : 2</t>
+  </si>
+  <si>
     <t>gateways : 1</t>
   </si>
   <si>
     <t>osi : 2</t>
   </si>
   <si>
+    <t>capacity planning : 1</t>
+  </si>
+  <si>
     <t>planning : 1</t>
   </si>
   <si>
     <t>protocols : 1</t>
   </si>
   <si>
+    <t>software development : 2</t>
+  </si>
+  <si>
     <t>automation : 2</t>
   </si>
   <si>
+    <t>systems analyst : 1</t>
+  </si>
+  <si>
+    <t>technical support : 1</t>
+  </si>
+  <si>
     <t>costing : 1</t>
   </si>
   <si>
+    <t>systems engineer : 1</t>
+  </si>
+  <si>
     <t>engineer : 1</t>
   </si>
   <si>
+    <t>object oriented : 1</t>
+  </si>
+  <si>
     <t>design : 1</t>
   </si>
   <si>
-    <t>embedded : 1</t>
-  </si>
-  <si>
-    <t>financial services : 1</t>
-  </si>
-  <si>
-    <t>oracle dba : 10</t>
-  </si>
-  <si>
-    <t>redhat linux : 7</t>
-  </si>
-  <si>
-    <t>oracle applications : 1</t>
-  </si>
-  <si>
-    <t>production support : 2</t>
-  </si>
-  <si>
-    <t>performance monitoring : 1</t>
-  </si>
-  <si>
-    <t>system administrator : 2</t>
-  </si>
-  <si>
-    <t>oracle databases : 2</t>
-  </si>
-  <si>
-    <t>cloud computing : 1</t>
-  </si>
-  <si>
-    <t>sql tuning : 2</t>
-  </si>
-  <si>
-    <t>windows servers : 1</t>
+    <t>embedded software : 2</t>
   </si>
   <si>
     <t>red hat linux : 2</t>
   </si>
   <si>
-    <t>unix scripting : 1</t>
-  </si>
-  <si>
-    <t>elastic search : 1</t>
-  </si>
-  <si>
-    <t>oracle 12c : 3</t>
-  </si>
-  <si>
-    <t>high availability : 1</t>
-  </si>
-  <si>
-    <t>data quality : 1</t>
-  </si>
-  <si>
-    <t>oracle rac : 2</t>
-  </si>
-  <si>
     <t>it : 2</t>
   </si>
   <si>
-    <t>oracle fusion : 1</t>
-  </si>
-  <si>
-    <t>security clearance : 2</t>
-  </si>
-  <si>
     <t>unix shell scripting : 1</t>
   </si>
   <si>
-    <t>data capture : 1</t>
-  </si>
-  <si>
-    <t>database tuning : 1</t>
-  </si>
-  <si>
-    <t>trouble shooting : 1</t>
-  </si>
-  <si>
-    <t>windows server : 1</t>
-  </si>
-  <si>
-    <t>general ledger : 1</t>
-  </si>
-  <si>
-    <t>disaster recovery : 1</t>
-  </si>
-  <si>
-    <t>system administration : 1</t>
-  </si>
-  <si>
     <t>front end : 1</t>
   </si>
   <si>
-    <t>business objects : 1</t>
-  </si>
-  <si>
     <t>pl/sql : 1</t>
   </si>
   <si>
-    <t>cisco routers : 1</t>
-  </si>
-  <si>
-    <t>system analysis : 1</t>
-  </si>
-  <si>
-    <t>customer support : 1</t>
-  </si>
-  <si>
-    <t>network management : 2</t>
-  </si>
-  <si>
-    <t>embedded software : 1</t>
+    <t>project : 1</t>
+  </si>
+  <si>
+    <t>analysis : 1</t>
+  </si>
+  <si>
+    <t>git : 1</t>
+  </si>
+  <si>
+    <t>sql : 1</t>
   </si>
   <si>
     <t>databases : 2</t>
   </si>
   <si>
-    <t>git : 1</t>
-  </si>
-  <si>
-    <t>sql : 1</t>
-  </si>
-  <si>
-    <t>project : 1</t>
-  </si>
-  <si>
-    <t>analysis : 1</t>
-  </si>
-  <si>
-    <t>35.71</t>
+    <t>27.77</t>
   </si>
   <si>
     <t>regulations : 2</t>
@@ -978,7 +1074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K186"/>
+  <dimension ref="A1:K218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1046,19 +1142,19 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>237</v>
       </c>
       <c r="I2" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="K2" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1066,10 +1162,10 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="H3" t="s">
-        <v>205</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1077,7 +1173,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1085,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1093,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>203</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1994,6 +2090,166 @@
     <row r="186" spans="5:5">
       <c r="E186" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="187" spans="5:5">
+      <c r="E187" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="188" spans="5:5">
+      <c r="E188" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="189" spans="5:5">
+      <c r="E189" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="190" spans="5:5">
+      <c r="E190" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="191" spans="5:5">
+      <c r="E191" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="192" spans="5:5">
+      <c r="E192" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="193" spans="5:5">
+      <c r="E193" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="194" spans="5:5">
+      <c r="E194" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="195" spans="5:5">
+      <c r="E195" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="196" spans="5:5">
+      <c r="E196" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="197" spans="5:5">
+      <c r="E197" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="198" spans="5:5">
+      <c r="E198" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="199" spans="5:5">
+      <c r="E199" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="200" spans="5:5">
+      <c r="E200" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="201" spans="5:5">
+      <c r="E201" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="202" spans="5:5">
+      <c r="E202" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="203" spans="5:5">
+      <c r="E203" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="204" spans="5:5">
+      <c r="E204" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="205" spans="5:5">
+      <c r="E205" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="206" spans="5:5">
+      <c r="E206" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="207" spans="5:5">
+      <c r="E207" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="208" spans="5:5">
+      <c r="E208" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="209" spans="5:5">
+      <c r="E209" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="210" spans="5:5">
+      <c r="E210" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="211" spans="5:5">
+      <c r="E211" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="212" spans="5:5">
+      <c r="E212" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="213" spans="5:5">
+      <c r="E213" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="214" spans="5:5">
+      <c r="E214" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="215" spans="5:5">
+      <c r="E215" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="216" spans="5:5">
+      <c r="E216" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="217" spans="5:5">
+      <c r="E217" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="218" spans="5:5">
+      <c r="E218" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixed for finding the name of experience
</commit_message>
<xml_diff>
--- a/upload_files/BK_746_2-converted__text.xlsx
+++ b/upload_files/BK_746_2-converted__text.xlsx
@@ -67,7 +67,7 @@
     <t>electronics : 1</t>
   </si>
   <si>
-    <t>contract : 23</t>
+    <t>contract : 22</t>
   </si>
   <si>
     <t>energy : 2</t>
@@ -79,7 +79,7 @@
     <t>tv : 2</t>
   </si>
   <si>
-    <t>financial services : 3</t>
+    <t>financial services : 4</t>
   </si>
   <si>
     <t>international : 2</t>
@@ -91,22 +91,22 @@
     <t>systems : 12</t>
   </si>
   <si>
-    <t>telecommunications : 3</t>
-  </si>
-  <si>
-    <t>oracle dba : 53</t>
-  </si>
-  <si>
-    <t>dba : 73</t>
+    <t>telecommunications : 4</t>
+  </si>
+  <si>
+    <t>oracle dba : 48</t>
+  </si>
+  <si>
+    <t>dba : 75</t>
   </si>
   <si>
     <t>consultant : 8</t>
   </si>
   <si>
-    <t>unix : 7</t>
-  </si>
-  <si>
-    <t>system administrator : 7</t>
+    <t>unix : 6</t>
+  </si>
+  <si>
+    <t>system administrator : 8</t>
   </si>
   <si>
     <t>administrator : 5</t>
@@ -124,34 +124,34 @@
     <t>admin : 1</t>
   </si>
   <si>
-    <t>oracle : 130</t>
-  </si>
-  <si>
-    <t>oracle applications : 3</t>
-  </si>
-  <si>
-    <t>middleware : 4</t>
-  </si>
-  <si>
-    <t>oem : 19</t>
+    <t>oracle : 136</t>
+  </si>
+  <si>
+    <t>oracle applications : 2</t>
+  </si>
+  <si>
+    <t>middleware : 2</t>
+  </si>
+  <si>
+    <t>oem : 17</t>
   </si>
   <si>
     <t>monitor : 1</t>
   </si>
   <si>
-    <t>oracle databases : 8</t>
-  </si>
-  <si>
-    <t>databases : 28</t>
-  </si>
-  <si>
-    <t>patching : 8</t>
-  </si>
-  <si>
-    <t>tuning : 30</t>
-  </si>
-  <si>
-    <t>monitoring : 16</t>
+    <t>oracle databases : 7</t>
+  </si>
+  <si>
+    <t>databases : 29</t>
+  </si>
+  <si>
+    <t>patching : 10</t>
+  </si>
+  <si>
+    <t>tuning : 27</t>
+  </si>
+  <si>
+    <t>monitoring : 13</t>
   </si>
   <si>
     <t>rman : 20</t>
@@ -160,10 +160,10 @@
     <t>testing : 10</t>
   </si>
   <si>
-    <t>redhat linux : 16</t>
-  </si>
-  <si>
-    <t>linux : 14</t>
+    <t>redhat linux : 15</t>
+  </si>
+  <si>
+    <t>linux : 15</t>
   </si>
   <si>
     <t>vmware : 7</t>
@@ -178,16 +178,16 @@
     <t>project : 13</t>
   </si>
   <si>
-    <t>migration : 13</t>
+    <t>migration : 14</t>
   </si>
   <si>
     <t>tools : 3</t>
   </si>
   <si>
-    <t>database : 29</t>
-  </si>
-  <si>
-    <t>backup : 7</t>
+    <t>database : 30</t>
+  </si>
+  <si>
+    <t>backup : 8</t>
   </si>
   <si>
     <t>recovery : 5</t>
@@ -196,10 +196,10 @@
     <t>production : 15</t>
   </si>
   <si>
-    <t>development : 21</t>
-  </si>
-  <si>
-    <t>production support : 5</t>
+    <t>development : 20</t>
+  </si>
+  <si>
+    <t>production support : 4</t>
   </si>
   <si>
     <t>ibm : 6</t>
@@ -208,10 +208,10 @@
     <t>aix : 7</t>
   </si>
   <si>
-    <t>servers : 41</t>
-  </si>
-  <si>
-    <t>azure : 1</t>
+    <t>servers : 42</t>
+  </si>
+  <si>
+    <t>azure : 2</t>
   </si>
   <si>
     <t>oracle 12c : 9</t>
@@ -226,7 +226,7 @@
     <t>security : 6</t>
   </si>
   <si>
-    <t>installation : 8</t>
+    <t>installation : 9</t>
   </si>
   <si>
     <t>soa : 2</t>
@@ -235,13 +235,13 @@
     <t>performance monitoring : 2</t>
   </si>
   <si>
-    <t>windows : 7</t>
+    <t>windows : 6</t>
   </si>
   <si>
     <t>database management : 1</t>
   </si>
   <si>
-    <t>management : 24</t>
+    <t>management : 26</t>
   </si>
   <si>
     <t>sales : 2</t>
@@ -250,31 +250,31 @@
     <t>oracle rac : 6</t>
   </si>
   <si>
-    <t>symantec : 2</t>
+    <t>symantec : 1</t>
   </si>
   <si>
     <t>automated : 1</t>
   </si>
   <si>
-    <t>configuration : 16</t>
-  </si>
-  <si>
-    <t>sqlserver : 5</t>
+    <t>configuration : 14</t>
+  </si>
+  <si>
+    <t>sqlserver : 4</t>
   </si>
   <si>
     <t>training : 5</t>
   </si>
   <si>
-    <t>sql : 12</t>
-  </si>
-  <si>
-    <t>rackspace : 2</t>
-  </si>
-  <si>
-    <t>aws : 5</t>
-  </si>
-  <si>
-    <t>oracle database : 6</t>
+    <t>sql : 13</t>
+  </si>
+  <si>
+    <t>rackspace : 1</t>
+  </si>
+  <si>
+    <t>aws : 4</t>
+  </si>
+  <si>
+    <t>oracle database : 7</t>
   </si>
   <si>
     <t>warehouse : 2</t>
@@ -283,7 +283,7 @@
     <t>aws cloud : 1</t>
   </si>
   <si>
-    <t>cloud computing : 2</t>
+    <t>cloud computing : 1</t>
   </si>
   <si>
     <t>informatica : 4</t>
@@ -298,10 +298,10 @@
     <t>grid : 9</t>
   </si>
   <si>
-    <t>toad : 6</t>
-  </si>
-  <si>
-    <t>sql tuning : 5</t>
+    <t>toad : 5</t>
+  </si>
+  <si>
+    <t>sql tuning : 3</t>
   </si>
   <si>
     <t>windows servers : 4</t>
@@ -313,7 +313,7 @@
     <t>rest : 1</t>
   </si>
   <si>
-    <t>unix scripting : 4</t>
+    <t>unix scripting : 5</t>
   </si>
   <si>
     <t>scripting : 6</t>
@@ -340,7 +340,7 @@
     <t>global : 3</t>
   </si>
   <si>
-    <t>ovm : 1</t>
+    <t>ovm : 2</t>
   </si>
   <si>
     <t>ux : 1</t>
@@ -358,7 +358,7 @@
     <t>data quality : 2</t>
   </si>
   <si>
-    <t>audit : 4</t>
+    <t>audit : 3</t>
   </si>
   <si>
     <t>regulations : 1</t>
@@ -391,7 +391,7 @@
     <t>apex : 2</t>
   </si>
   <si>
-    <t>performance tuning : 2</t>
+    <t>performance tuning : 3</t>
   </si>
   <si>
     <t>data migration : 1</t>
@@ -433,7 +433,7 @@
     <t>security clearance : 5</t>
   </si>
   <si>
-    <t>oracle fusion : 2</t>
+    <t>oracle fusion : 1</t>
   </si>
   <si>
     <t>fusion : 1</t>
@@ -451,7 +451,7 @@
     <t>incident management : 1</t>
   </si>
   <si>
-    <t>sla : 2</t>
+    <t>sla : 1</t>
   </si>
   <si>
     <t>install : 1</t>
@@ -523,7 +523,7 @@
     <t>database tuning : 2</t>
   </si>
   <si>
-    <t>trouble shooting : 2</t>
+    <t>trouble shooting : 1</t>
   </si>
   <si>
     <t>statistics : 1</t>
@@ -553,7 +553,7 @@
     <t>veritas : 4</t>
   </si>
   <si>
-    <t>windows server : 2</t>
+    <t>windows server : 1</t>
   </si>
   <si>
     <t>credit risk : 1</t>
@@ -568,7 +568,7 @@
     <t>peoplesoft : 1</t>
   </si>
   <si>
-    <t>sybase : 1</t>
+    <t>sybase : 2</t>
   </si>
   <si>
     <t>software : 9</t>
@@ -589,7 +589,7 @@
     <t>business objects : 2</t>
   </si>
   <si>
-    <t>business continuity : 1</t>
+    <t>business continuity : 2</t>
   </si>
   <si>
     <t>cluster : 6</t>
@@ -604,7 +604,7 @@
     <t>tivoli : 2</t>
   </si>
   <si>
-    <t>network management : 7</t>
+    <t>network management : 9</t>
   </si>
   <si>
     <t>tcp : 3</t>
@@ -655,7 +655,7 @@
     <t>osi : 2</t>
   </si>
   <si>
-    <t>capacity planning : 1</t>
+    <t>capacity planning : 2</t>
   </si>
   <si>
     <t>planning : 1</t>
@@ -676,7 +676,7 @@
     <t>technical support : 1</t>
   </si>
   <si>
-    <t>costing : 1</t>
+    <t>costing : 2</t>
   </si>
   <si>
     <t>systems engineer : 1</t>
@@ -694,6 +694,9 @@
     <t>embedded software : 2</t>
   </si>
   <si>
+    <t>it services : 1</t>
+  </si>
+  <si>
     <t>red hat linux : 2</t>
   </si>
   <si>
@@ -703,25 +706,22 @@
     <t>unix shell scripting : 1</t>
   </si>
   <si>
-    <t>front end : 1</t>
-  </si>
-  <si>
-    <t>pl/sql : 1</t>
+    <t>pl/sql : 2</t>
   </si>
   <si>
     <t>project : 1</t>
   </si>
   <si>
+    <t>sql : 1</t>
+  </si>
+  <si>
     <t>analysis : 1</t>
   </si>
   <si>
+    <t>databases : 2</t>
+  </si>
+  <si>
     <t>git : 1</t>
-  </si>
-  <si>
-    <t>sql : 1</t>
-  </si>
-  <si>
-    <t>databases : 2</t>
   </si>
   <si>
     <t>27.77</t>

</xml_diff>

<commit_message>
Time Improved for Algo
</commit_message>
<xml_diff>
--- a/upload_files/BK_746_2-converted__text.xlsx
+++ b/upload_files/BK_746_2-converted__text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="224">
   <si>
     <t>CV ID</t>
   </si>
@@ -55,7 +55,7 @@
     <t>text.txt</t>
   </si>
   <si>
-    <t>26.80</t>
+    <t>27.15</t>
   </si>
   <si>
     <t>image processing : 1</t>
@@ -76,24 +76,15 @@
     <t>plc : 4</t>
   </si>
   <si>
-    <t>tv : 2</t>
-  </si>
-  <si>
     <t>financial services : 4</t>
   </si>
   <si>
-    <t>international : 2</t>
-  </si>
-  <si>
     <t>network : 8</t>
   </si>
   <si>
     <t>systems : 12</t>
   </si>
   <si>
-    <t>telecommunications : 4</t>
-  </si>
-  <si>
     <t>oracle dba : 48</t>
   </si>
   <si>
@@ -175,9 +166,6 @@
     <t>administration : 6</t>
   </si>
   <si>
-    <t>project : 13</t>
-  </si>
-  <si>
     <t>migration : 14</t>
   </si>
   <si>
@@ -196,9 +184,6 @@
     <t>production : 15</t>
   </si>
   <si>
-    <t>development : 20</t>
-  </si>
-  <si>
     <t>production support : 4</t>
   </si>
   <si>
@@ -235,18 +220,12 @@
     <t>performance monitoring : 2</t>
   </si>
   <si>
-    <t>windows : 6</t>
-  </si>
-  <si>
     <t>database management : 1</t>
   </si>
   <si>
     <t>management : 26</t>
   </si>
   <si>
-    <t>sales : 2</t>
-  </si>
-  <si>
     <t>oracle rac : 6</t>
   </si>
   <si>
@@ -262,9 +241,6 @@
     <t>sqlserver : 4</t>
   </si>
   <si>
-    <t>training : 5</t>
-  </si>
-  <si>
     <t>sql : 13</t>
   </si>
   <si>
@@ -361,9 +337,6 @@
     <t>audit : 3</t>
   </si>
   <si>
-    <t>regulations : 1</t>
-  </si>
-  <si>
     <t>data architect : 1</t>
   </si>
   <si>
@@ -463,9 +436,6 @@
     <t>hardware : 1</t>
   </si>
   <si>
-    <t>engineering : 1</t>
-  </si>
-  <si>
     <t>ms sql : 1</t>
   </si>
   <si>
@@ -571,9 +541,6 @@
     <t>sybase : 2</t>
   </si>
   <si>
-    <t>software : 9</t>
-  </si>
-  <si>
     <t>enterprise manager : 2</t>
   </si>
   <si>
@@ -610,9 +577,6 @@
     <t>tcp : 3</t>
   </si>
   <si>
-    <t>ip : 3</t>
-  </si>
-  <si>
     <t>cisco routers : 2</t>
   </si>
   <si>
@@ -637,9 +601,6 @@
     <t>c : 2</t>
   </si>
   <si>
-    <t>communication : 1</t>
-  </si>
-  <si>
     <t>system analysis : 2</t>
   </si>
   <si>
@@ -700,37 +661,28 @@
     <t>red hat linux : 2</t>
   </si>
   <si>
-    <t>it : 2</t>
-  </si>
-  <si>
     <t>unix shell scripting : 1</t>
   </si>
   <si>
     <t>pl/sql : 2</t>
   </si>
   <si>
-    <t>project : 1</t>
+    <t>git : 1</t>
+  </si>
+  <si>
+    <t>analysis : 1</t>
   </si>
   <si>
     <t>sql : 1</t>
   </si>
   <si>
-    <t>analysis : 1</t>
-  </si>
-  <si>
     <t>databases : 2</t>
   </si>
   <si>
-    <t>git : 1</t>
-  </si>
-  <si>
-    <t>27.77</t>
-  </si>
-  <si>
-    <t>regulations : 2</t>
-  </si>
-  <si>
-    <t>20.0</t>
+    <t>28.57</t>
+  </si>
+  <si>
+    <t>14.28</t>
   </si>
   <si>
     <t>0.0</t>
@@ -1074,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K218"/>
+  <dimension ref="A1:K204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1142,19 +1094,19 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="K2" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1162,10 +1114,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H3" t="s">
-        <v>92</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1173,7 +1122,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1181,16 +1130,13 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="E7" t="s">
@@ -2180,76 +2126,6 @@
     <row r="204" spans="5:5">
       <c r="E204" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="205" spans="5:5">
-      <c r="E205" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="206" spans="5:5">
-      <c r="E206" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="207" spans="5:5">
-      <c r="E207" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="208" spans="5:5">
-      <c r="E208" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="209" spans="5:5">
-      <c r="E209" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="210" spans="5:5">
-      <c r="E210" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="211" spans="5:5">
-      <c r="E211" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="212" spans="5:5">
-      <c r="E212" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="213" spans="5:5">
-      <c r="E213" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="214" spans="5:5">
-      <c r="E214" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="215" spans="5:5">
-      <c r="E215" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="216" spans="5:5">
-      <c r="E216" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="217" spans="5:5">
-      <c r="E217" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="218" spans="5:5">
-      <c r="E218" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>